<commit_message>
excel atrasos nuevo cambio
</commit_message>
<xml_diff>
--- a/seguimientoAtrasos.xlsx
+++ b/seguimientoAtrasos.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Liceo Siete\OneDrive\Documentos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Liceo Siete\OneDrive\Documentos\atrasos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0386615E-DA77-4AB3-9D7B-B212DC932141}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4C8A0D4-6190-48EA-969C-AE34AB86FE56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{053382FF-8DDD-4AFD-A1F1-97B33F62579F}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="314">
   <si>
     <t>Ord</t>
   </si>
@@ -1106,6 +1106,9 @@
     <t>apoderado manda correo comprometiendo 
 que asistirá a hacer aseo el viernes, 
 pero no asiste el día comprometio</t>
+  </si>
+  <si>
+    <t>nuevo cambio</t>
   </si>
 </sst>
 </file>
@@ -3817,7 +3820,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="L6" sqref="L6"/>
+      <selection pane="topRight" activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -3978,7 +3981,9 @@
       <c r="J6" s="191" t="s">
         <v>63</v>
       </c>
-      <c r="K6" s="3"/>
+      <c r="K6" s="3" t="s">
+        <v>313</v>
+      </c>
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
     </row>

</xml_diff>